<commit_message>
AI example of the Glossary
</commit_message>
<xml_diff>
--- a/TestDocs/E2e_tests_R4D.xlsx
+++ b/TestDocs/E2e_tests_R4D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EnyFood\Random4Dinner\TestDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A82A71-86D4-45BF-BD00-7352FFDD7FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B7CF54-4A70-4893-A5B1-9BC486EB9215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44100" yWindow="795" windowWidth="31650" windowHeight="12330" activeTab="1" xr2:uid="{45BE1B39-84B1-47C3-9973-4B355870E5A1}"/>
+    <workbookView xWindow="-44100" yWindow="795" windowWidth="36525" windowHeight="18945" activeTab="1" xr2:uid="{45BE1B39-84B1-47C3-9973-4B355870E5A1}"/>
   </bookViews>
   <sheets>
     <sheet name="E2E" sheetId="1" r:id="rId1"/>
@@ -598,9 +598,6 @@
     <t>The method of measuring the quantity of the Ingredient is selected</t>
   </si>
   <si>
-    <t>Additional panel isn't useful</t>
-  </si>
-  <si>
     <t>Tap the proportions stepper to decrease the amount (-1)</t>
   </si>
   <si>
@@ -641,6 +638,9 @@
   </si>
   <si>
     <t>The counting logic isn't clear</t>
+  </si>
+  <si>
+    <t>Additional panel isn't useful for the User</t>
   </si>
 </sst>
 </file>
@@ -1691,6 +1691,48 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1721,65 +1763,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2311,17 +2311,17 @@
       <c r="B1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="80"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="94"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
@@ -2333,16 +2333,16 @@
       <c r="E2" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="81" t="s">
+      <c r="F2" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="83"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="97"/>
     </row>
     <row r="3" spans="1:13" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
@@ -2352,16 +2352,16 @@
       <c r="E3" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="84" t="s">
+      <c r="F3" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="86"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="100"/>
     </row>
     <row r="4" spans="1:13" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
@@ -2373,16 +2373,16 @@
       <c r="E4" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="84" t="s">
+      <c r="F4" s="98" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
-      <c r="M4" s="86"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="100"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
@@ -2395,39 +2395,39 @@
       <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="90" t="s">
+      <c r="A7" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="93" t="s">
+      <c r="B7" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="86" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="77" t="s">
+      <c r="E7" s="91" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="91"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="97"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="87"/>
       <c r="D8" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="77"/>
+      <c r="E8" s="91"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="92"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="98"/>
+      <c r="A9" s="82"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="77"/>
+      <c r="E9" s="91"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
@@ -2436,11 +2436,11 @@
       <c r="D10" s="47"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="89"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="79"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
@@ -2485,11 +2485,11 @@
       <c r="D15" s="38"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="88"/>
-      <c r="C16" s="88"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
       <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2547,11 +2547,11 @@
       <c r="D21" s="38"/>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="99" t="s">
+      <c r="A22" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="100"/>
-      <c r="C22" s="100"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="90"/>
       <c r="D22" s="40"/>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2692,11 +2692,11 @@
       <c r="C34" s="54"/>
     </row>
     <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="87" t="s">
+      <c r="A35" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="88"/>
-      <c r="C35" s="89"/>
+      <c r="B35" s="78"/>
+      <c r="C35" s="79"/>
     </row>
     <row r="36" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
@@ -2776,11 +2776,11 @@
       <c r="C42" s="66"/>
     </row>
     <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="87" t="s">
+      <c r="A43" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="88"/>
-      <c r="C43" s="89"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="79"/>
     </row>
     <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
@@ -3315,6 +3315,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="F3:M3"/>
+    <mergeCell ref="F4:M4"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A43:C43"/>
     <mergeCell ref="A7:A9"/>
@@ -3323,11 +3328,6 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A22:C22"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="F2:M2"/>
-    <mergeCell ref="F3:M3"/>
-    <mergeCell ref="F4:M4"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
@@ -3585,7 +3585,7 @@
   <dimension ref="A1:M74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3603,17 +3603,17 @@
       <c r="B1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="80"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="94"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
@@ -3625,16 +3625,16 @@
       <c r="E2" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="81" t="s">
+      <c r="F2" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="83"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="97"/>
     </row>
     <row r="3" spans="1:13" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
@@ -3644,16 +3644,16 @@
       <c r="E3" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="84" t="s">
+      <c r="F3" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="86"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="100"/>
     </row>
     <row r="4" spans="1:13" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
@@ -3665,16 +3665,16 @@
       <c r="E4" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="84" t="s">
+      <c r="F4" s="98" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
-      <c r="M4" s="86"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="100"/>
     </row>
     <row r="5" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
@@ -3687,39 +3687,39 @@
       <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="103" t="s">
+      <c r="B7" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="104" t="s">
+      <c r="C7" s="103" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="77" t="s">
+      <c r="E7" s="91" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="91"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="105"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="104"/>
       <c r="D8" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="77"/>
+      <c r="E8" s="91"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="92"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="106"/>
+      <c r="A9" s="82"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="105"/>
       <c r="D9" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="E9" s="77"/>
+      <c r="E9" s="91"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
@@ -3727,11 +3727,11 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="89"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="79"/>
     </row>
     <row r="12" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
@@ -3788,11 +3788,11 @@
       <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="88"/>
-      <c r="C16" s="88"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
       <c r="D16" s="30"/>
       <c r="E16" s="19"/>
     </row>
@@ -3865,11 +3865,11 @@
       <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="99" t="s">
+      <c r="A22" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="100"/>
-      <c r="C22" s="101"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="106"/>
       <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -4063,11 +4063,11 @@
       <c r="E35" s="19"/>
     </row>
     <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="87" t="s">
+      <c r="A36" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="88"/>
-      <c r="C36" s="89"/>
+      <c r="B36" s="78"/>
+      <c r="C36" s="79"/>
       <c r="E36" s="19"/>
     </row>
     <row r="37" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -4138,7 +4138,7 @@
         <v>26</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>84</v>
@@ -4169,11 +4169,11 @@
       <c r="E43" s="19"/>
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="87" t="s">
+      <c r="A44" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="88"/>
-      <c r="C44" s="89"/>
+      <c r="B44" s="78"/>
+      <c r="C44" s="79"/>
       <c r="E44" s="19"/>
     </row>
     <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4184,7 +4184,7 @@
         <v>37</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>169</v>
@@ -4319,7 +4319,7 @@
         <v>120</v>
       </c>
       <c r="C54" s="75" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D54" s="41" t="s">
         <v>83</v>
@@ -4552,12 +4552,12 @@
         <v>83</v>
       </c>
       <c r="E69" s="19" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B70" s="76" t="s">
         <v>185</v>
@@ -4572,36 +4572,36 @@
     </row>
     <row r="71" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B71" s="76" t="s">
+        <v>188</v>
+      </c>
+      <c r="C71" s="74" t="s">
         <v>189</v>
-      </c>
-      <c r="C71" s="74" t="s">
-        <v>190</v>
       </c>
       <c r="D71" s="40" t="s">
         <v>83</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B72" s="76" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C72" s="74" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D72" s="40" t="s">
         <v>83</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4612,13 +4612,13 @@
         <v>153</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D73" s="40" t="s">
         <v>84</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4629,7 +4629,7 @@
         <v>154</v>
       </c>
       <c r="C74" s="49" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D74" s="40" t="s">
         <v>83</v>
@@ -4638,6 +4638,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A44:C44"/>
     <mergeCell ref="E1:M1"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="F3:M3"/>
@@ -4646,11 +4651,6 @@
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="E7:E9"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A44:C44"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>